<commit_message>
Sarah's csv files loaded in SQL subdir of Code
</commit_message>
<xml_diff>
--- a/Code/IPython/car_sales.xlsx
+++ b/Code/IPython/car_sales.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="sales_table" sheetId="1" r:id="rId1"/>
@@ -318,8 +318,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -365,7 +375,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -385,6 +395,11 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -404,6 +419,11 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -736,7 +756,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection sqref="A1:G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3083,8 +3103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3631,7 +3651,7 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection sqref="A1:C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4765,8 +4785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>